<commit_message>
files for co-authors review
</commit_message>
<xml_diff>
--- a/Data/qPCR_data_dominance1.xlsx
+++ b/Data/qPCR_data_dominance1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive-105793286447324059497/My Drive/RStudio/Dominance Project/DomRegen_Data_Repository/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinvarholick/Documents/GitHub/AcomysDominance_2022_Data_Results/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91968C56-4D67-A948-A412-F5C96B02D49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8618E96F-5461-6047-84A6-3F7DC37ACE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="500" windowWidth="18880" windowHeight="21100" activeTab="1" xr2:uid="{B2A07D43-BBCC-41F3-AA36-57966DAC006D}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{B2A07D43-BBCC-41F3-AA36-57966DAC006D}"/>
   </bookViews>
   <sheets>
     <sheet name="AllRuns" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3526" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3634" uniqueCount="130">
   <si>
     <t>plate</t>
   </si>
@@ -414,6 +414,18 @@
   <si>
     <t>Cyp11a1</t>
   </si>
+  <si>
+    <t>990342-1</t>
+  </si>
+  <si>
+    <t>990342-2</t>
+  </si>
+  <si>
+    <t>1001363-1</t>
+  </si>
+  <si>
+    <t>1001363-2</t>
+  </si>
 </sst>
 </file>
 
@@ -422,7 +434,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.00;\-###0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,7 +445,7 @@
     <font>
       <sz val="8.25"/>
       <name val="Microsoft Sans Serif"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -445,7 +457,14 @@
       <b/>
       <sz val="8.25"/>
       <name val="Microsoft Sans Serif"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -468,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -488,6 +507,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6279C1CC-AD46-47F8-8CA6-3067D56C50B5}">
-  <dimension ref="A1:E618"/>
+  <dimension ref="A1:E636"/>
   <sheetViews>
     <sheetView topLeftCell="A591" workbookViewId="0">
-      <selection activeCell="A618" sqref="A551:E618"/>
+      <selection activeCell="A619" sqref="A619:A636"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11276,6 +11296,306 @@
       </c>
       <c r="E618" s="6">
         <v>19.096737873802827</v>
+      </c>
+    </row>
+    <row r="619" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A619" s="7">
+        <v>9</v>
+      </c>
+      <c r="B619" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C619" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D619" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E619" s="2">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="620" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A620" s="7">
+        <v>9</v>
+      </c>
+      <c r="B620" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C620" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D620" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E620" s="2">
+        <v>17.55</v>
+      </c>
+    </row>
+    <row r="621" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A621" s="7">
+        <v>9</v>
+      </c>
+      <c r="B621" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C621" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D621" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E621" s="2">
+        <v>17.72</v>
+      </c>
+    </row>
+    <row r="622" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A622" s="7">
+        <v>9</v>
+      </c>
+      <c r="B622" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C622" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D622" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E622" s="2">
+        <v>19.53</v>
+      </c>
+    </row>
+    <row r="623" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A623" s="7">
+        <v>9</v>
+      </c>
+      <c r="B623" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C623" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D623" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E623" s="2">
+        <v>19.09</v>
+      </c>
+    </row>
+    <row r="624" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A624" s="7">
+        <v>9</v>
+      </c>
+      <c r="B624" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C624" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D624" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E624" s="2">
+        <v>19.010000000000002</v>
+      </c>
+    </row>
+    <row r="625" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A625" s="7">
+        <v>9</v>
+      </c>
+      <c r="B625" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C625" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D625" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E625" s="2">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="626" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A626" s="7">
+        <v>9</v>
+      </c>
+      <c r="B626" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C626" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D626" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E626" s="2">
+        <v>17.14</v>
+      </c>
+    </row>
+    <row r="627" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A627" s="7">
+        <v>9</v>
+      </c>
+      <c r="B627" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C627" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D627" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E627" s="2">
+        <v>17.21</v>
+      </c>
+    </row>
+    <row r="628" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A628" s="7">
+        <v>9</v>
+      </c>
+      <c r="B628" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C628" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D628" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E628" s="2">
+        <v>18.05</v>
+      </c>
+    </row>
+    <row r="629" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A629" s="7">
+        <v>9</v>
+      </c>
+      <c r="B629" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C629" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D629" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E629" s="2">
+        <v>17.89</v>
+      </c>
+    </row>
+    <row r="630" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A630" s="7">
+        <v>9</v>
+      </c>
+      <c r="B630" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C630" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D630" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E630" s="2">
+        <v>18.079999999999998</v>
+      </c>
+    </row>
+    <row r="631" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A631" s="7">
+        <v>9</v>
+      </c>
+      <c r="B631" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C631" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D631" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E631" s="2"/>
+    </row>
+    <row r="632" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A632" s="7">
+        <v>9</v>
+      </c>
+      <c r="B632" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C632" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D632" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E632" s="2"/>
+    </row>
+    <row r="633" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A633" s="7">
+        <v>9</v>
+      </c>
+      <c r="B633" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C633" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D633" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E633" s="2"/>
+    </row>
+    <row r="634" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A634" s="7">
+        <v>9</v>
+      </c>
+      <c r="B634" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C634" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D634" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E634" s="2">
+        <v>22.09</v>
+      </c>
+    </row>
+    <row r="635" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A635" s="7">
+        <v>9</v>
+      </c>
+      <c r="B635" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C635" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D635" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E635" s="2">
+        <v>19.97</v>
+      </c>
+    </row>
+    <row r="636" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A636" s="7">
+        <v>9</v>
+      </c>
+      <c r="B636" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C636" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D636" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E636" s="2">
+        <v>18.670000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -11286,10 +11606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D510C51D-F1FA-49F0-8AAA-CECF22E519B2}">
-  <dimension ref="A1:E556"/>
+  <dimension ref="A1:E574"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A478" workbookViewId="0">
-      <selection activeCell="E493" sqref="E493:E495"/>
+    <sheetView tabSelected="1" topLeftCell="A539" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="G570" sqref="G570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20724,6 +21044,306 @@
         <v>19.096737873802827</v>
       </c>
     </row>
+    <row r="557" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A557">
+        <v>9</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C557" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D557" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E557" s="2">
+        <v>18.504747959478401</v>
+      </c>
+    </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A558">
+        <v>9</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C558" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D558" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E558" s="2">
+        <v>17.552963617593001</v>
+      </c>
+    </row>
+    <row r="559" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A559">
+        <v>9</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C559" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D559" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E559" s="2">
+        <v>17.718575768376301</v>
+      </c>
+    </row>
+    <row r="560" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A560">
+        <v>9</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C560" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D560" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E560" s="2">
+        <v>19.529693995837501</v>
+      </c>
+    </row>
+    <row r="561" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A561">
+        <v>9</v>
+      </c>
+      <c r="B561" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C561" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D561" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E561" s="2">
+        <v>19.0915799689739</v>
+      </c>
+    </row>
+    <row r="562" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A562">
+        <v>9</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C562" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D562" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E562" s="2">
+        <v>19.0107303777976</v>
+      </c>
+    </row>
+    <row r="563" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A563">
+        <v>9</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C563" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D563" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E563" s="2">
+        <v>17.296210665377401</v>
+      </c>
+    </row>
+    <row r="564" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A564">
+        <v>9</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C564" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D564" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E564" s="2">
+        <v>17.135714952526701</v>
+      </c>
+    </row>
+    <row r="565" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A565">
+        <v>9</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C565" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D565" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E565" s="2">
+        <v>17.209629118767399</v>
+      </c>
+    </row>
+    <row r="566" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A566">
+        <v>9</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C566" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D566" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E566" s="2">
+        <v>18.045892707321102</v>
+      </c>
+    </row>
+    <row r="567" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A567">
+        <v>9</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C567" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D567" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E567" s="2">
+        <v>17.887365019339601</v>
+      </c>
+    </row>
+    <row r="568" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A568">
+        <v>9</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C568" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D568" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E568" s="2">
+        <v>18.081928493476799</v>
+      </c>
+    </row>
+    <row r="569" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A569">
+        <v>9</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C569" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D569" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E569" s="2"/>
+    </row>
+    <row r="570" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A570">
+        <v>9</v>
+      </c>
+      <c r="B570" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C570" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D570" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E570" s="2"/>
+    </row>
+    <row r="571" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A571">
+        <v>9</v>
+      </c>
+      <c r="B571" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C571" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D571" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E571" s="2"/>
+    </row>
+    <row r="572" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A572">
+        <v>9</v>
+      </c>
+      <c r="B572" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C572" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D572" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E572" s="2">
+        <v>22.090157989788999</v>
+      </c>
+    </row>
+    <row r="573" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A573">
+        <v>9</v>
+      </c>
+      <c r="B573" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C573" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D573" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E573" s="2">
+        <v>19.968349952821601</v>
+      </c>
+    </row>
+    <row r="574" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A574">
+        <v>9</v>
+      </c>
+      <c r="B574" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C574" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D574" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E574" s="2">
+        <v>18.665255716402999</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E494">
     <sortCondition ref="C1:C494"/>

</xml_diff>